<commit_message>
made slight changes, forgot to drop extra index column in output file
</commit_message>
<xml_diff>
--- a/tut03/small_longest_subsequence.xlsx
+++ b/tut03/small_longest_subsequence.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cs384_2022\Documents\GitHub\CS384_2022\tut03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e57038ad28c6e6dc/Documents/New folder/2001ME35_2022/tut03/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_992ED33B335594C8D7DCA1007CF80F9817A477DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -92,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,19 +437,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="14" max="14" width="28.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -526,7 +535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -565,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.02</v>
       </c>
@@ -604,7 +613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.03</v>
       </c>
@@ -643,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.04</v>
       </c>
@@ -682,7 +691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.05</v>
       </c>
@@ -721,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.06</v>
       </c>
@@ -760,7 +769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -799,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.08</v>
       </c>
@@ -838,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.09</v>
       </c>
@@ -868,7 +877,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.1</v>
       </c>
@@ -898,7 +907,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.11</v>
       </c>
@@ -928,7 +937,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.12</v>
       </c>
@@ -958,7 +967,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.13</v>
       </c>
@@ -988,7 +997,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.14000000000000001</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.15</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.16</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.17</v>
       </c>
@@ -1108,7 +1117,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.18</v>
       </c>
@@ -1138,7 +1147,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.19</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.2</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>+3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.21</v>
       </c>
@@ -1228,7 +1237,7 @@
         <v>+3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.22</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.23</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>+4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.24</v>
       </c>
@@ -1318,7 +1327,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.25</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>+3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.26</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.27</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>+3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.28000000000000003</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>+4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.28999999999999998</v>
       </c>
@@ -1468,7 +1477,7 @@
         <v>+4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.3</v>
       </c>
@@ -1498,7 +1507,7 @@
         <v>+3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.31</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.32</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.33</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>+2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.34</v>
       </c>

</xml_diff>